<commit_message>
refactor: Remove Windows build and run scripts, update CMake for Qt5 only
- Deleted `build.bat` and `run_dbc_viewer.bat` scripts to streamline the build process.
- Updated `CMakeLists.txt` to exclusively find and link against Qt5, removing fallback for Qt6.
- Adjusted `README.md` to reflect the removal of Windows-specific build instructions and clarified system requirements.
- Enhanced Excel export functionality in `dbcexcelconverter` and `dbcparser` to include document title support.
</commit_message>
<xml_diff>
--- a/20240105_C5_PP_ADCANFD_FLSDR_V04.xlsx
+++ b/20240105_C5_PP_ADCANFD_FLSDR_V04.xlsx
@@ -451,6 +451,9 @@
       <c r="Z4" s="2">
         <v>20</v>
       </c>
+      <c r="AA4" s="2">
+        <v>10</v>
+      </c>
       <c r="AC4" t="inlineStr" s="2">
         <is>
           <t>FDR</t>
@@ -936,6 +939,9 @@
       <c r="Z12" s="2">
         <v>20</v>
       </c>
+      <c r="AA12" s="2">
+        <v>10</v>
+      </c>
       <c r="AC12" t="inlineStr" s="2">
         <is>
           <t>FLSDR</t>
@@ -2001,6 +2007,9 @@
       </c>
       <c r="Z30" s="2">
         <v>20</v>
+      </c>
+      <c r="AA30" s="2">
+        <v>10</v>
       </c>
       <c r="AC30" t="inlineStr" s="2">
         <is>
@@ -4328,6 +4337,9 @@
       <c r="Z66" s="2">
         <v>20</v>
       </c>
+      <c r="AA66" s="2">
+        <v>10</v>
+      </c>
       <c r="AC66" t="inlineStr" s="2">
         <is>
           <t>GW</t>
@@ -6759,6 +6771,9 @@
       <c r="Z105" s="2">
         <v>20</v>
       </c>
+      <c r="AA105" s="2">
+        <v>10</v>
+      </c>
       <c r="AC105" t="inlineStr" s="2">
         <is>
           <t>RLSDR</t>
@@ -7134,6 +7149,9 @@
       </c>
       <c r="Z111" s="2">
         <v>20</v>
+      </c>
+      <c r="AA111" s="2">
+        <v>10</v>
       </c>
       <c r="AC111" t="inlineStr" s="2">
         <is>

</xml_diff>

<commit_message>
fix: Adjust xSplit attribute in Excel XML generation for improved layout
- Updated the xSplit attribute in the XML generation logic to enhance the worksheet layout in the Excel export.
- Ensured the change aligns with recent updates to the message structure, improving overall data representation.
</commit_message>
<xml_diff>
--- a/20240105_C5_PP_ADCANFD_FLSDR_V04.xlsx
+++ b/20240105_C5_PP_ADCANFD_FLSDR_V04.xlsx
@@ -208,7 +208,7 @@
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,7 +716,7 @@
   <dimension ref="A1:AE122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8404,7 +8404,7 @@
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8890,7 +8890,7 @@
   <dimension ref="A1:AE94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14890,7 +14890,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -16237,7 +16237,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -17584,7 +17584,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18931,7 +18931,7 @@
   <dimension ref="A1:AE19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="1" zoomScale="70">
-      <pane xSplit="11" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
feat: Add raw range handling for CAN signals and enhance validation checks
- Introduced methods to set and clear raw range values for CAN signals, allowing for the import of hex bus min/max values from Excel.
- Updated the DbcExcelConverter to parse and set raw range values during Excel import.
- Enhanced validation logic to check if raw min/max values are within valid signed/unsigned ranges and added error reporting for invalid values.
- Implemented a new utility function to parse hex values as signed integers for validation purposes.
</commit_message>
<xml_diff>
--- a/20240105_C5_PP_ADCANFD_FLSDR_V04.xlsx
+++ b/20240105_C5_PP_ADCANFD_FLSDR_V04.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jingyang\Downloads\1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C6A277-C4BF-4875-84D1-6DF027C5F6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28800" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="主页" sheetId="1" r:id="rId1"/>
@@ -22,13 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1242" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243" uniqueCount="324">
   <si>
     <r>
       <rPr>
         <sz val="24"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>4D</t>
     </r>
@@ -44,7 +38,7 @@
       <rPr>
         <sz val="24"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <charset val="134"/>
       </rPr>
       <t>GPAL Ares-F(C)R6C</t>
     </r>
@@ -52,7 +46,7 @@
       <rPr>
         <sz val="24"/>
         <rFont val="Times New Roman"/>
-        <family val="1"/>
+        <charset val="134"/>
       </rPr>
       <t xml:space="preserve">
 </t>
@@ -1127,8 +1121,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -1139,13 +1139,13 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="24"/>
@@ -1153,17 +1153,163 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="24"/>
       <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1188,8 +1334,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1212,11 +1544,253 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1230,28 +1804,62 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1509,208 +2117,69 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H16"/>
+      <selection activeCell="A1" sqref="A1:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-    </row>
-    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-    </row>
+    <row r="1" s="4" customFormat="1" ht="24" customHeight="1" spans="1:1">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" ht="24" customHeight="1"/>
+    <row r="3" ht="24" customHeight="1"/>
+    <row r="4" ht="24" customHeight="1"/>
+    <row r="5" ht="24" customHeight="1"/>
+    <row r="6" ht="24" customHeight="1"/>
+    <row r="7" ht="24" customHeight="1"/>
+    <row r="8" ht="24" customHeight="1"/>
+    <row r="9" ht="24" customHeight="1"/>
+    <row r="10" ht="24" customHeight="1"/>
+    <row r="11" ht="24" customHeight="1"/>
+    <row r="12" ht="24" customHeight="1"/>
+    <row r="13" ht="24" customHeight="1"/>
+    <row r="14" ht="24" customHeight="1"/>
+    <row r="15" ht="24" customHeight="1"/>
+    <row r="16" ht="24" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:H16"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="48" customWidth="1"/>
     <col min="4" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="24" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1731,26 +2200,27 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AE156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="T36" activePane="bottomRight" state="frozen"/>
+      <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="N91" sqref="N91"/>
+      <selection pane="bottomRight" activeCell="W100" sqref="W100"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="22" customWidth="1"/>
     <col min="3" max="7" width="11" customWidth="1"/>
@@ -1762,7 +2232,7 @@
     <col min="31" max="31" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" s="1" customFormat="1" ht="30" customHeight="1" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1857,7 +2327,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="2" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:12">
       <c r="A2" s="2" t="s">
         <v>38</v>
       </c>
@@ -1895,19 +2365,8 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
+    <row r="3" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A3" s="2"/>
       <c r="M3" s="3" t="s">
         <v>45</v>
       </c>
@@ -1957,7 +2416,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="4" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>52</v>
       </c>
@@ -1992,19 +2451,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
+    <row r="5" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A5" s="2"/>
       <c r="M5" s="3" t="s">
         <v>55</v>
       </c>
@@ -2054,7 +2502,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="6" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A6" s="2" t="s">
         <v>58</v>
       </c>
@@ -2089,19 +2537,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="8"/>
+    <row r="7" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A7" s="2"/>
       <c r="M7" s="3" t="s">
         <v>61</v>
       </c>
@@ -2148,19 +2585,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="8"/>
+    <row r="8" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M8" s="3" t="s">
         <v>64</v>
       </c>
@@ -2207,19 +2632,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="8"/>
+    <row r="9" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M9" s="3" t="s">
         <v>67</v>
       </c>
@@ -2266,19 +2679,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
+    <row r="10" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M10" s="3" t="s">
         <v>69</v>
       </c>
@@ -2325,19 +2726,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="8"/>
+    <row r="11" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M11" s="3" t="s">
         <v>71</v>
       </c>
@@ -2384,7 +2773,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="12" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -2419,19 +2808,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
+    <row r="13" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A13" s="2"/>
       <c r="M13" s="3" t="s">
         <v>76</v>
       </c>
@@ -2478,19 +2856,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
+    <row r="14" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M14" s="3" t="s">
         <v>77</v>
       </c>
@@ -2537,19 +2903,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
+    <row r="15" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M15" s="3" t="s">
         <v>78</v>
       </c>
@@ -2596,19 +2950,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:31" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+    <row r="16" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M16" s="3" t="s">
         <v>79</v>
       </c>
@@ -2655,19 +2997,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+    <row r="17" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M17" s="3" t="s">
         <v>81</v>
       </c>
@@ -2714,19 +3044,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:27" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+    <row r="18" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M18" s="3" t="s">
         <v>83</v>
       </c>
@@ -2773,19 +3091,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:27" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+    <row r="19" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M19" s="3" t="s">
         <v>85</v>
       </c>
@@ -2832,19 +3138,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
+    <row r="20" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M20" s="3" t="s">
         <v>87</v>
       </c>
@@ -2891,19 +3185,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
+    <row r="21" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M21" s="3" t="s">
         <v>89</v>
       </c>
@@ -2950,19 +3232,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
+    <row r="22" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M22" s="3" t="s">
         <v>91</v>
       </c>
@@ -3009,19 +3279,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
+    <row r="23" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M23" s="3" t="s">
         <v>92</v>
       </c>
@@ -3068,7 +3326,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="24" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A24" s="2" t="s">
         <v>93</v>
       </c>
@@ -3103,19 +3361,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
+    <row r="25" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A25" s="2"/>
       <c r="M25" s="3" t="s">
         <v>95</v>
       </c>
@@ -3159,7 +3406,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="26" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A26" s="2" t="s">
         <v>97</v>
       </c>
@@ -3194,19 +3441,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
+    <row r="27" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A27" s="2"/>
       <c r="M27" s="3" t="s">
         <v>97</v>
       </c>
@@ -3238,7 +3474,7 @@
         <v>0</v>
       </c>
       <c r="X27" s="3">
-        <v>1.8446744073709601E+19</v>
+        <v>1.84467440737096e+19</v>
       </c>
       <c r="Y27" s="3" t="s">
         <v>49</v>
@@ -3250,7 +3486,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="28" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A28" s="2" t="s">
         <v>102</v>
       </c>
@@ -3285,19 +3521,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="8"/>
+    <row r="29" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A29" s="2"/>
       <c r="M29" s="3" t="s">
         <v>102</v>
       </c>
@@ -3329,7 +3554,7 @@
         <v>0</v>
       </c>
       <c r="X29" s="3">
-        <v>1.8446744073709601E+19</v>
+        <v>1.84467440737096e+19</v>
       </c>
       <c r="Y29" s="3" t="s">
         <v>49</v>
@@ -3341,7 +3566,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="30" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A30" s="2" t="s">
         <v>104</v>
       </c>
@@ -3376,19 +3601,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
+    <row r="31" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A31" s="2"/>
       <c r="M31" s="3" t="s">
         <v>107</v>
       </c>
@@ -3435,19 +3649,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="8"/>
+    <row r="32" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M32" s="3" t="s">
         <v>108</v>
       </c>
@@ -3494,19 +3696,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="8"/>
+    <row r="33" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M33" s="3" t="s">
         <v>109</v>
       </c>
@@ -3553,19 +3743,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="8"/>
+    <row r="34" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M34" s="3" t="s">
         <v>110</v>
       </c>
@@ -3612,19 +3790,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
+    <row r="35" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M35" s="3" t="s">
         <v>111</v>
       </c>
@@ -3671,7 +3837,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="36" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A36" s="2" t="s">
         <v>112</v>
       </c>
@@ -3706,19 +3872,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="8"/>
+    <row r="37" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A37" s="2"/>
       <c r="M37" s="3" t="s">
         <v>115</v>
       </c>
@@ -3762,19 +3917,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="8"/>
+    <row r="38" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M38" s="3" t="s">
         <v>116</v>
       </c>
@@ -3824,19 +3967,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="39" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="8"/>
+    <row r="39" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M39" s="3" t="s">
         <v>119</v>
       </c>
@@ -3880,19 +4011,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="8"/>
+    <row r="40" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M40" s="3" t="s">
         <v>121</v>
       </c>
@@ -3939,19 +4058,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="8"/>
+    <row r="41" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M41" s="3" t="s">
         <v>123</v>
       </c>
@@ -3995,19 +4102,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
+    <row r="42" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M42" s="3" t="s">
         <v>124</v>
       </c>
@@ -4051,19 +4146,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="8"/>
+    <row r="43" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M43" s="3" t="s">
         <v>125</v>
       </c>
@@ -4113,7 +4196,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="44" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A44" s="2" t="s">
         <v>128</v>
       </c>
@@ -4148,19 +4231,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-      <c r="F45" s="8"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
+    <row r="45" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A45" s="2"/>
       <c r="M45" s="3" t="s">
         <v>130</v>
       </c>
@@ -4204,19 +4276,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="8"/>
+    <row r="46" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M46" s="3" t="s">
         <v>131</v>
       </c>
@@ -4260,19 +4320,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="8"/>
+    <row r="47" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M47" s="3" t="s">
         <v>132</v>
       </c>
@@ -4322,19 +4370,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:31" s="3" customFormat="1" ht="75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
+    <row r="48" s="3" customFormat="1" ht="75" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M48" s="3" t="s">
         <v>134</v>
       </c>
@@ -4384,7 +4420,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="49" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="49" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A49" s="2" t="s">
         <v>138</v>
       </c>
@@ -4419,19 +4455,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:31" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
-      <c r="E50" s="8"/>
-      <c r="F50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="8"/>
+    <row r="50" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A50" s="2"/>
       <c r="M50" s="3" t="s">
         <v>140</v>
       </c>
@@ -4481,19 +4506,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:31" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8"/>
-      <c r="F51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="8"/>
+    <row r="51" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M51" s="3" t="s">
         <v>144</v>
       </c>
@@ -4543,19 +4556,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:31" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="8"/>
-      <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="8"/>
+    <row r="52" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M52" s="3" t="s">
         <v>147</v>
       </c>
@@ -4605,7 +4606,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="53" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A53" s="2" t="s">
         <v>150</v>
       </c>
@@ -4640,19 +4641,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="8"/>
-      <c r="C54" s="8"/>
-      <c r="D54" s="8"/>
-      <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="8"/>
+    <row r="54" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A54" s="2"/>
       <c r="M54" s="3" t="s">
         <v>152</v>
       </c>
@@ -4699,19 +4689,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8"/>
-      <c r="F55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="8"/>
+    <row r="55" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M55" s="3" t="s">
         <v>154</v>
       </c>
@@ -4761,19 +4739,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="56" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="8"/>
+    <row r="56" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M56" s="3" t="s">
         <v>156</v>
       </c>
@@ -4820,19 +4786,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="57" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="8"/>
-      <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="8"/>
+    <row r="57" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M57" s="3" t="s">
         <v>157</v>
       </c>
@@ -4879,7 +4833,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="58" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="58" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A58" s="2" t="s">
         <v>158</v>
       </c>
@@ -4914,19 +4868,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:31" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
-      <c r="B59" s="8"/>
-      <c r="C59" s="8"/>
-      <c r="D59" s="8"/>
-      <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="8"/>
+    <row r="59" s="3" customFormat="1" ht="90" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A59" s="2"/>
       <c r="M59" s="3" t="s">
         <v>160</v>
       </c>
@@ -4976,19 +4919,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="60" spans="1:31" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="8"/>
-      <c r="B60" s="8"/>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8"/>
+    <row r="60" s="3" customFormat="1" ht="90" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M60" s="3" t="s">
         <v>163</v>
       </c>
@@ -5038,19 +4969,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="61" spans="1:31" s="3" customFormat="1" ht="90" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="8"/>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8"/>
-      <c r="E61" s="8"/>
-      <c r="F61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="8"/>
+    <row r="61" s="3" customFormat="1" ht="75" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M61" s="3" t="s">
         <v>165</v>
       </c>
@@ -5100,19 +5019,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="8"/>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-      <c r="E62" s="8"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
+    <row r="62" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M62" s="3" t="s">
         <v>168</v>
       </c>
@@ -5162,19 +5069,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="63" spans="1:31" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="8"/>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-      <c r="E63" s="8"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
+    <row r="63" s="3" customFormat="1" ht="90" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M63" s="3" t="s">
         <v>171</v>
       </c>
@@ -5224,19 +5119,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="64" spans="1:31" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="8"/>
-      <c r="B64" s="8"/>
-      <c r="C64" s="8"/>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8"/>
-      <c r="F64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="8"/>
+    <row r="64" s="3" customFormat="1" ht="90" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M64" s="3" t="s">
         <v>173</v>
       </c>
@@ -5286,19 +5169,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="65" spans="1:31" s="3" customFormat="1" ht="105" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
-      <c r="C65" s="8"/>
-      <c r="D65" s="8"/>
-      <c r="E65" s="8"/>
-      <c r="F65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="8"/>
+    <row r="65" s="3" customFormat="1" ht="90" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M65" s="3" t="s">
         <v>175</v>
       </c>
@@ -5348,7 +5219,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="66" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="66" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A66" s="2" t="s">
         <v>178</v>
       </c>
@@ -5383,19 +5254,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
-      <c r="B67" s="8"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="8"/>
-      <c r="E67" s="8"/>
-      <c r="F67" s="8"/>
-      <c r="G67" s="8"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="8"/>
+    <row r="67" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A67" s="2"/>
       <c r="M67" s="3" t="s">
         <v>180</v>
       </c>
@@ -5442,19 +5302,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="68" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
-      <c r="B68" s="8"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="8"/>
-      <c r="F68" s="8"/>
-      <c r="G68" s="8"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="8"/>
+    <row r="68" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M68" s="3" t="s">
         <v>181</v>
       </c>
@@ -5501,19 +5349,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="69" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
-      <c r="B69" s="8"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="8"/>
-      <c r="F69" s="8"/>
-      <c r="G69" s="8"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="8"/>
+    <row r="69" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M69" s="3" t="s">
         <v>182</v>
       </c>
@@ -5560,19 +5396,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
+    <row r="70" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M70" s="3" t="s">
         <v>183</v>
       </c>
@@ -5619,19 +5443,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="71" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="8"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="8"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="8"/>
+    <row r="71" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M71" s="3" t="s">
         <v>184</v>
       </c>
@@ -5678,7 +5490,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="72" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A72" s="2" t="s">
         <v>185</v>
       </c>
@@ -5713,19 +5525,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
-      <c r="B73" s="8"/>
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="E73" s="8"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="8"/>
+    <row r="73" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A73" s="2"/>
       <c r="M73" s="3" t="s">
         <v>187</v>
       </c>
@@ -5772,19 +5573,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
-      <c r="E74" s="8"/>
-      <c r="F74" s="8"/>
-      <c r="G74" s="8"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="8"/>
+    <row r="74" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M74" s="3" t="s">
         <v>189</v>
       </c>
@@ -5831,19 +5620,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="75" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="8"/>
-      <c r="B75" s="8"/>
-      <c r="C75" s="8"/>
-      <c r="D75" s="8"/>
-      <c r="E75" s="8"/>
-      <c r="F75" s="8"/>
-      <c r="G75" s="8"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="8"/>
+    <row r="75" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M75" s="3" t="s">
         <v>191</v>
       </c>
@@ -5890,19 +5667,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="76" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="8"/>
-      <c r="B76" s="8"/>
-      <c r="C76" s="8"/>
-      <c r="D76" s="8"/>
-      <c r="E76" s="8"/>
-      <c r="F76" s="8"/>
-      <c r="G76" s="8"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="8"/>
-      <c r="L76" s="8"/>
+    <row r="76" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M76" s="3" t="s">
         <v>193</v>
       </c>
@@ -5949,19 +5714,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="8"/>
-      <c r="B77" s="8"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="8"/>
-      <c r="E77" s="8"/>
-      <c r="F77" s="8"/>
-      <c r="G77" s="8"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="8"/>
+    <row r="77" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M77" s="3" t="s">
         <v>195</v>
       </c>
@@ -6008,19 +5761,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="78" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="8"/>
-      <c r="B78" s="8"/>
-      <c r="C78" s="8"/>
-      <c r="D78" s="8"/>
-      <c r="E78" s="8"/>
-      <c r="F78" s="8"/>
-      <c r="G78" s="8"/>
-      <c r="H78" s="8"/>
-      <c r="I78" s="8"/>
-      <c r="J78" s="8"/>
-      <c r="K78" s="8"/>
-      <c r="L78" s="8"/>
+    <row r="78" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M78" s="3" t="s">
         <v>197</v>
       </c>
@@ -6067,19 +5808,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="79" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
-      <c r="C79" s="8"/>
-      <c r="D79" s="8"/>
-      <c r="E79" s="8"/>
-      <c r="F79" s="8"/>
-      <c r="G79" s="8"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="8"/>
+    <row r="79" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M79" s="3" t="s">
         <v>199</v>
       </c>
@@ -6126,19 +5855,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
-      <c r="C80" s="8"/>
-      <c r="D80" s="8"/>
-      <c r="E80" s="8"/>
-      <c r="F80" s="8"/>
-      <c r="G80" s="8"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="8"/>
+    <row r="80" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M80" s="3" t="s">
         <v>201</v>
       </c>
@@ -6185,7 +5902,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" s="2" customFormat="1" ht="24" customHeight="1" spans="1:11">
       <c r="A81" s="2" t="s">
         <v>203</v>
       </c>
@@ -6220,19 +5937,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="8"/>
-      <c r="C82" s="8"/>
-      <c r="D82" s="8"/>
-      <c r="E82" s="8"/>
-      <c r="F82" s="8"/>
-      <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
-      <c r="L82" s="8"/>
+    <row r="82" s="3" customFormat="1" outlineLevel="1" spans="1:27">
+      <c r="A82" s="2"/>
       <c r="M82" s="3" t="s">
         <v>205</v>
       </c>
@@ -6279,19 +5985,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="83" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="8"/>
-      <c r="B83" s="8"/>
-      <c r="C83" s="8"/>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8"/>
-      <c r="F83" s="8"/>
-      <c r="G83" s="8"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="8"/>
-      <c r="K83" s="8"/>
-      <c r="L83" s="8"/>
+    <row r="83" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M83" s="3" t="s">
         <v>207</v>
       </c>
@@ -6338,19 +6032,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="84" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="8"/>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
-      <c r="E84" s="8"/>
-      <c r="F84" s="8"/>
-      <c r="G84" s="8"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8"/>
-      <c r="L84" s="8"/>
+    <row r="84" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M84" s="3" t="s">
         <v>209</v>
       </c>
@@ -6397,19 +6079,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="85" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="8"/>
-      <c r="B85" s="8"/>
-      <c r="C85" s="8"/>
-      <c r="D85" s="8"/>
-      <c r="E85" s="8"/>
-      <c r="F85" s="8"/>
-      <c r="G85" s="8"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
-      <c r="L85" s="8"/>
+    <row r="85" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M85" s="3" t="s">
         <v>211</v>
       </c>
@@ -6456,19 +6126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="8"/>
-      <c r="B86" s="8"/>
-      <c r="C86" s="8"/>
-      <c r="D86" s="8"/>
-      <c r="E86" s="8"/>
-      <c r="F86" s="8"/>
-      <c r="G86" s="8"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="8"/>
+    <row r="86" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M86" s="3" t="s">
         <v>213</v>
       </c>
@@ -6515,19 +6173,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="87" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="8"/>
-      <c r="B87" s="8"/>
-      <c r="C87" s="8"/>
-      <c r="D87" s="8"/>
-      <c r="E87" s="8"/>
-      <c r="F87" s="8"/>
-      <c r="G87" s="8"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8"/>
-      <c r="L87" s="8"/>
+    <row r="87" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M87" s="3" t="s">
         <v>215</v>
       </c>
@@ -6574,19 +6220,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="88" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="8"/>
-      <c r="B88" s="8"/>
-      <c r="C88" s="8"/>
-      <c r="D88" s="8"/>
-      <c r="E88" s="8"/>
-      <c r="F88" s="8"/>
-      <c r="G88" s="8"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
-      <c r="L88" s="8"/>
+    <row r="88" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M88" s="3" t="s">
         <v>217</v>
       </c>
@@ -6633,19 +6267,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="89" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="8"/>
-      <c r="B89" s="8"/>
-      <c r="C89" s="8"/>
-      <c r="D89" s="8"/>
-      <c r="E89" s="8"/>
-      <c r="F89" s="8"/>
-      <c r="G89" s="8"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="8"/>
+    <row r="89" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M89" s="3" t="s">
         <v>219</v>
       </c>
@@ -6692,7 +6314,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="90" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" s="2" customFormat="1" ht="24" customHeight="1" spans="1:11">
       <c r="A90" s="2" t="s">
         <v>221</v>
       </c>
@@ -6727,19 +6349,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
-      <c r="B91" s="8"/>
-      <c r="C91" s="8"/>
-      <c r="D91" s="8"/>
-      <c r="E91" s="8"/>
-      <c r="F91" s="8"/>
-      <c r="G91" s="8"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
-      <c r="L91" s="8"/>
+    <row r="91" s="3" customFormat="1" outlineLevel="1" spans="1:27">
+      <c r="A91" s="2"/>
       <c r="M91" s="3" t="s">
         <v>223</v>
       </c>
@@ -6786,19 +6397,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="92" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="8"/>
-      <c r="B92" s="8"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="8"/>
-      <c r="E92" s="8"/>
-      <c r="F92" s="8"/>
-      <c r="G92" s="8"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-      <c r="L92" s="8"/>
+    <row r="92" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M92" s="3" t="s">
         <v>224</v>
       </c>
@@ -6845,19 +6444,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="93" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="8"/>
-      <c r="B93" s="8"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="8"/>
-      <c r="E93" s="8"/>
-      <c r="F93" s="8"/>
-      <c r="G93" s="8"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="8"/>
+    <row r="93" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M93" s="3" t="s">
         <v>225</v>
       </c>
@@ -6904,19 +6491,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="94" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="8"/>
-      <c r="E94" s="8"/>
-      <c r="F94" s="8"/>
-      <c r="G94" s="8"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
-      <c r="L94" s="8"/>
+    <row r="94" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M94" s="3" t="s">
         <v>226</v>
       </c>
@@ -6963,19 +6538,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="95" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="8"/>
-      <c r="B95" s="8"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="8"/>
-      <c r="E95" s="8"/>
-      <c r="F95" s="8"/>
-      <c r="G95" s="8"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="8"/>
+    <row r="95" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M95" s="3" t="s">
         <v>227</v>
       </c>
@@ -7022,19 +6585,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="96" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="8"/>
-      <c r="B96" s="8"/>
-      <c r="C96" s="8"/>
-      <c r="D96" s="8"/>
-      <c r="E96" s="8"/>
-      <c r="F96" s="8"/>
-      <c r="G96" s="8"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="8"/>
+    <row r="96" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M96" s="3" t="s">
         <v>228</v>
       </c>
@@ -7081,19 +6632,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="97" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="8"/>
-      <c r="B97" s="8"/>
-      <c r="C97" s="8"/>
-      <c r="D97" s="8"/>
-      <c r="E97" s="8"/>
-      <c r="F97" s="8"/>
-      <c r="G97" s="8"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
-      <c r="L97" s="8"/>
+    <row r="97" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M97" s="3" t="s">
         <v>229</v>
       </c>
@@ -7140,19 +6679,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="8"/>
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
-      <c r="F98" s="8"/>
-      <c r="G98" s="8"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-      <c r="K98" s="8"/>
-      <c r="L98" s="8"/>
+    <row r="98" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M98" s="3" t="s">
         <v>230</v>
       </c>
@@ -7199,7 +6726,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" s="2" customFormat="1" ht="24" customHeight="1" spans="1:11">
       <c r="A99" s="2" t="s">
         <v>231</v>
       </c>
@@ -7234,19 +6761,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="7"/>
-      <c r="B100" s="8"/>
-      <c r="C100" s="8"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-      <c r="G100" s="8"/>
-      <c r="H100" s="8"/>
-      <c r="I100" s="8"/>
-      <c r="J100" s="8"/>
-      <c r="K100" s="8"/>
-      <c r="L100" s="8"/>
+    <row r="100" s="3" customFormat="1" outlineLevel="1" spans="1:29">
+      <c r="A100" s="2"/>
       <c r="M100" s="3" t="s">
         <v>233</v>
       </c>
@@ -7278,7 +6794,7 @@
         <v>0</v>
       </c>
       <c r="W100" s="3">
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="X100" s="3">
         <v>255</v>
@@ -7287,25 +6803,19 @@
         <v>49</v>
       </c>
       <c r="Z100" s="3" t="s">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="AA100" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="101" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="8"/>
-      <c r="B101" s="8"/>
-      <c r="C101" s="8"/>
-      <c r="D101" s="8"/>
-      <c r="E101" s="8"/>
-      <c r="F101" s="8"/>
-      <c r="G101" s="8"/>
-      <c r="H101" s="8"/>
-      <c r="I101" s="8"/>
-      <c r="J101" s="8"/>
-      <c r="K101" s="8"/>
-      <c r="L101" s="8"/>
+      <c r="AB100" s="3">
+        <v>-10</v>
+      </c>
+      <c r="AC100" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="101" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M101" s="3" t="s">
         <v>234</v>
       </c>
@@ -7352,19 +6862,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="102" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="8"/>
-      <c r="B102" s="8"/>
-      <c r="C102" s="8"/>
-      <c r="D102" s="8"/>
-      <c r="E102" s="8"/>
-      <c r="F102" s="8"/>
-      <c r="G102" s="8"/>
-      <c r="H102" s="8"/>
-      <c r="I102" s="8"/>
-      <c r="J102" s="8"/>
-      <c r="K102" s="8"/>
-      <c r="L102" s="8"/>
+    <row r="102" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M102" s="3" t="s">
         <v>235</v>
       </c>
@@ -7411,19 +6909,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="103" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="8"/>
-      <c r="B103" s="8"/>
-      <c r="C103" s="8"/>
-      <c r="D103" s="8"/>
-      <c r="E103" s="8"/>
-      <c r="F103" s="8"/>
-      <c r="G103" s="8"/>
-      <c r="H103" s="8"/>
-      <c r="I103" s="8"/>
-      <c r="J103" s="8"/>
-      <c r="K103" s="8"/>
-      <c r="L103" s="8"/>
+    <row r="103" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M103" s="3" t="s">
         <v>236</v>
       </c>
@@ -7470,19 +6956,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="104" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="8"/>
-      <c r="B104" s="8"/>
-      <c r="C104" s="8"/>
-      <c r="D104" s="8"/>
-      <c r="E104" s="8"/>
-      <c r="F104" s="8"/>
-      <c r="G104" s="8"/>
-      <c r="H104" s="8"/>
-      <c r="I104" s="8"/>
-      <c r="J104" s="8"/>
-      <c r="K104" s="8"/>
-      <c r="L104" s="8"/>
+    <row r="104" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M104" s="3" t="s">
         <v>237</v>
       </c>
@@ -7529,19 +7003,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="105" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="8"/>
-      <c r="B105" s="8"/>
-      <c r="C105" s="8"/>
-      <c r="D105" s="8"/>
-      <c r="E105" s="8"/>
-      <c r="F105" s="8"/>
-      <c r="G105" s="8"/>
-      <c r="H105" s="8"/>
-      <c r="I105" s="8"/>
-      <c r="J105" s="8"/>
-      <c r="K105" s="8"/>
-      <c r="L105" s="8"/>
+    <row r="105" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M105" s="3" t="s">
         <v>238</v>
       </c>
@@ -7588,19 +7050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
-      <c r="B106" s="8"/>
-      <c r="C106" s="8"/>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8"/>
-      <c r="F106" s="8"/>
-      <c r="G106" s="8"/>
-      <c r="H106" s="8"/>
-      <c r="I106" s="8"/>
-      <c r="J106" s="8"/>
-      <c r="K106" s="8"/>
-      <c r="L106" s="8"/>
+    <row r="106" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M106" s="3" t="s">
         <v>239</v>
       </c>
@@ -7647,19 +7097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="107" spans="1:27" s="3" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="8"/>
-      <c r="B107" s="8"/>
-      <c r="C107" s="8"/>
-      <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8"/>
-      <c r="G107" s="8"/>
-      <c r="H107" s="8"/>
-      <c r="I107" s="8"/>
-      <c r="J107" s="8"/>
-      <c r="K107" s="8"/>
-      <c r="L107" s="8"/>
+    <row r="107" s="3" customFormat="1" outlineLevel="1" spans="13:27">
       <c r="M107" s="3" t="s">
         <v>240</v>
       </c>
@@ -7706,7 +7144,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="108" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="108" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A108" s="2" t="s">
         <v>241</v>
       </c>
@@ -7741,19 +7179,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
-      <c r="B109" s="8"/>
-      <c r="C109" s="8"/>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8"/>
-      <c r="F109" s="8"/>
-      <c r="G109" s="8"/>
-      <c r="H109" s="8"/>
-      <c r="I109" s="8"/>
-      <c r="J109" s="8"/>
-      <c r="K109" s="8"/>
-      <c r="L109" s="8"/>
+    <row r="109" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A109" s="2"/>
       <c r="M109" s="3" t="s">
         <v>243</v>
       </c>
@@ -7800,19 +7227,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="110" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
-      <c r="C110" s="8"/>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
-      <c r="F110" s="8"/>
-      <c r="G110" s="8"/>
-      <c r="H110" s="8"/>
-      <c r="I110" s="8"/>
-      <c r="J110" s="8"/>
-      <c r="K110" s="8"/>
-      <c r="L110" s="8"/>
+    <row r="110" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M110" s="3" t="s">
         <v>244</v>
       </c>
@@ -7859,19 +7274,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="111" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="8"/>
-      <c r="B111" s="8"/>
-      <c r="C111" s="8"/>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8"/>
-      <c r="F111" s="8"/>
-      <c r="G111" s="8"/>
-      <c r="H111" s="8"/>
-      <c r="I111" s="8"/>
-      <c r="J111" s="8"/>
-      <c r="K111" s="8"/>
-      <c r="L111" s="8"/>
+    <row r="111" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M111" s="3" t="s">
         <v>245</v>
       </c>
@@ -7918,19 +7321,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="112" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="8"/>
-      <c r="B112" s="8"/>
-      <c r="C112" s="8"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-      <c r="G112" s="8"/>
-      <c r="H112" s="8"/>
-      <c r="I112" s="8"/>
-      <c r="J112" s="8"/>
-      <c r="K112" s="8"/>
-      <c r="L112" s="8"/>
+    <row r="112" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M112" s="3" t="s">
         <v>246</v>
       </c>
@@ -7977,19 +7368,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="113" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="8"/>
-      <c r="B113" s="8"/>
-      <c r="C113" s="8"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-      <c r="G113" s="8"/>
-      <c r="H113" s="8"/>
-      <c r="I113" s="8"/>
-      <c r="J113" s="8"/>
-      <c r="K113" s="8"/>
-      <c r="L113" s="8"/>
+    <row r="113" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M113" s="3" t="s">
         <v>247</v>
       </c>
@@ -8036,19 +7415,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="114" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="8"/>
-      <c r="B114" s="8"/>
-      <c r="C114" s="8"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-      <c r="G114" s="8"/>
-      <c r="H114" s="8"/>
-      <c r="I114" s="8"/>
-      <c r="J114" s="8"/>
-      <c r="K114" s="8"/>
-      <c r="L114" s="8"/>
+    <row r="114" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M114" s="3" t="s">
         <v>248</v>
       </c>
@@ -8095,19 +7462,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="115" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="8"/>
-      <c r="B115" s="8"/>
-      <c r="C115" s="8"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
-      <c r="G115" s="8"/>
-      <c r="H115" s="8"/>
-      <c r="I115" s="8"/>
-      <c r="J115" s="8"/>
-      <c r="K115" s="8"/>
-      <c r="L115" s="8"/>
+    <row r="115" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M115" s="3" t="s">
         <v>249</v>
       </c>
@@ -8154,19 +7509,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="116" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="8"/>
-      <c r="B116" s="8"/>
-      <c r="C116" s="8"/>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8"/>
-      <c r="F116" s="8"/>
-      <c r="G116" s="8"/>
-      <c r="H116" s="8"/>
-      <c r="I116" s="8"/>
-      <c r="J116" s="8"/>
-      <c r="K116" s="8"/>
-      <c r="L116" s="8"/>
+    <row r="116" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M116" s="3" t="s">
         <v>250</v>
       </c>
@@ -8213,7 +7556,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="117" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="117" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A117" s="2" t="s">
         <v>251</v>
       </c>
@@ -8248,19 +7591,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A118" s="7"/>
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
-      <c r="D118" s="8"/>
-      <c r="E118" s="8"/>
-      <c r="F118" s="8"/>
-      <c r="G118" s="8"/>
-      <c r="H118" s="8"/>
-      <c r="I118" s="8"/>
-      <c r="J118" s="8"/>
-      <c r="K118" s="8"/>
-      <c r="L118" s="8"/>
+    <row r="118" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A118" s="2"/>
       <c r="M118" s="3" t="s">
         <v>253</v>
       </c>
@@ -8307,19 +7639,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="8"/>
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
-      <c r="D119" s="8"/>
-      <c r="E119" s="8"/>
-      <c r="F119" s="8"/>
-      <c r="G119" s="8"/>
-      <c r="H119" s="8"/>
-      <c r="I119" s="8"/>
-      <c r="J119" s="8"/>
-      <c r="K119" s="8"/>
-      <c r="L119" s="8"/>
+    <row r="119" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M119" s="3" t="s">
         <v>254</v>
       </c>
@@ -8366,19 +7686,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="120" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A120" s="8"/>
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
-      <c r="D120" s="8"/>
-      <c r="E120" s="8"/>
-      <c r="F120" s="8"/>
-      <c r="G120" s="8"/>
-      <c r="H120" s="8"/>
-      <c r="I120" s="8"/>
-      <c r="J120" s="8"/>
-      <c r="K120" s="8"/>
-      <c r="L120" s="8"/>
+    <row r="120" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M120" s="3" t="s">
         <v>255</v>
       </c>
@@ -8425,19 +7733,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="121" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A121" s="8"/>
-      <c r="B121" s="8"/>
-      <c r="C121" s="8"/>
-      <c r="D121" s="8"/>
-      <c r="E121" s="8"/>
-      <c r="F121" s="8"/>
-      <c r="G121" s="8"/>
-      <c r="H121" s="8"/>
-      <c r="I121" s="8"/>
-      <c r="J121" s="8"/>
-      <c r="K121" s="8"/>
-      <c r="L121" s="8"/>
+    <row r="121" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M121" s="3" t="s">
         <v>256</v>
       </c>
@@ -8484,19 +7780,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="122" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="8"/>
-      <c r="B122" s="8"/>
-      <c r="C122" s="8"/>
-      <c r="D122" s="8"/>
-      <c r="E122" s="8"/>
-      <c r="F122" s="8"/>
-      <c r="G122" s="8"/>
-      <c r="H122" s="8"/>
-      <c r="I122" s="8"/>
-      <c r="J122" s="8"/>
-      <c r="K122" s="8"/>
-      <c r="L122" s="8"/>
+    <row r="122" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M122" s="3" t="s">
         <v>257</v>
       </c>
@@ -8543,19 +7827,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="123" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A123" s="8"/>
-      <c r="B123" s="8"/>
-      <c r="C123" s="8"/>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8"/>
-      <c r="F123" s="8"/>
-      <c r="G123" s="8"/>
-      <c r="H123" s="8"/>
-      <c r="I123" s="8"/>
-      <c r="J123" s="8"/>
-      <c r="K123" s="8"/>
-      <c r="L123" s="8"/>
+    <row r="123" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M123" s="3" t="s">
         <v>258</v>
       </c>
@@ -8602,19 +7874,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="124" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="8"/>
-      <c r="B124" s="8"/>
-      <c r="C124" s="8"/>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8"/>
-      <c r="F124" s="8"/>
-      <c r="G124" s="8"/>
-      <c r="H124" s="8"/>
-      <c r="I124" s="8"/>
-      <c r="J124" s="8"/>
-      <c r="K124" s="8"/>
-      <c r="L124" s="8"/>
+    <row r="124" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M124" s="3" t="s">
         <v>259</v>
       </c>
@@ -8661,19 +7921,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="125" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="8"/>
-      <c r="B125" s="8"/>
-      <c r="C125" s="8"/>
-      <c r="D125" s="8"/>
-      <c r="E125" s="8"/>
-      <c r="F125" s="8"/>
-      <c r="G125" s="8"/>
-      <c r="H125" s="8"/>
-      <c r="I125" s="8"/>
-      <c r="J125" s="8"/>
-      <c r="K125" s="8"/>
-      <c r="L125" s="8"/>
+    <row r="125" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M125" s="3" t="s">
         <v>260</v>
       </c>
@@ -8720,7 +7968,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="126" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="126" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A126" s="2" t="s">
         <v>261</v>
       </c>
@@ -8755,19 +8003,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:31" s="3" customFormat="1" ht="45" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="7"/>
-      <c r="B127" s="8"/>
-      <c r="C127" s="8"/>
-      <c r="D127" s="8"/>
-      <c r="E127" s="8"/>
-      <c r="F127" s="8"/>
-      <c r="G127" s="8"/>
-      <c r="H127" s="8"/>
-      <c r="I127" s="8"/>
-      <c r="J127" s="8"/>
-      <c r="K127" s="8"/>
-      <c r="L127" s="8"/>
+    <row r="127" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A127" s="2"/>
       <c r="M127" s="3" t="s">
         <v>263</v>
       </c>
@@ -8817,19 +8054,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="128" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="8"/>
-      <c r="B128" s="8"/>
-      <c r="C128" s="8"/>
-      <c r="D128" s="8"/>
-      <c r="E128" s="8"/>
-      <c r="F128" s="8"/>
-      <c r="G128" s="8"/>
-      <c r="H128" s="8"/>
-      <c r="I128" s="8"/>
-      <c r="J128" s="8"/>
-      <c r="K128" s="8"/>
-      <c r="L128" s="8"/>
+    <row r="128" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:30">
       <c r="M128" s="3" t="s">
         <v>266</v>
       </c>
@@ -8879,19 +8104,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="129" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="8"/>
-      <c r="B129" s="8"/>
-      <c r="C129" s="8"/>
-      <c r="D129" s="8"/>
-      <c r="E129" s="8"/>
-      <c r="F129" s="8"/>
-      <c r="G129" s="8"/>
-      <c r="H129" s="8"/>
-      <c r="I129" s="8"/>
-      <c r="J129" s="8"/>
-      <c r="K129" s="8"/>
-      <c r="L129" s="8"/>
+    <row r="129" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:30">
       <c r="M129" s="3" t="s">
         <v>269</v>
       </c>
@@ -8941,19 +8154,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="130" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="8"/>
-      <c r="B130" s="8"/>
-      <c r="C130" s="8"/>
-      <c r="D130" s="8"/>
-      <c r="E130" s="8"/>
-      <c r="F130" s="8"/>
-      <c r="G130" s="8"/>
-      <c r="H130" s="8"/>
-      <c r="I130" s="8"/>
-      <c r="J130" s="8"/>
-      <c r="K130" s="8"/>
-      <c r="L130" s="8"/>
+    <row r="130" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M130" s="3" t="s">
         <v>273</v>
       </c>
@@ -9000,19 +8201,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="131" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="8"/>
-      <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
-      <c r="D131" s="8"/>
-      <c r="E131" s="8"/>
-      <c r="F131" s="8"/>
-      <c r="G131" s="8"/>
-      <c r="H131" s="8"/>
-      <c r="I131" s="8"/>
-      <c r="J131" s="8"/>
-      <c r="K131" s="8"/>
-      <c r="L131" s="8"/>
+    <row r="131" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:30">
       <c r="M131" s="3" t="s">
         <v>275</v>
       </c>
@@ -9062,19 +8251,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="132" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="8"/>
-      <c r="B132" s="8"/>
-      <c r="C132" s="8"/>
-      <c r="D132" s="8"/>
-      <c r="E132" s="8"/>
-      <c r="F132" s="8"/>
-      <c r="G132" s="8"/>
-      <c r="H132" s="8"/>
-      <c r="I132" s="8"/>
-      <c r="J132" s="8"/>
-      <c r="K132" s="8"/>
-      <c r="L132" s="8"/>
+    <row r="132" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:30">
       <c r="M132" s="3" t="s">
         <v>278</v>
       </c>
@@ -9124,19 +8301,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="133" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="8"/>
-      <c r="B133" s="8"/>
-      <c r="C133" s="8"/>
-      <c r="D133" s="8"/>
-      <c r="E133" s="8"/>
-      <c r="F133" s="8"/>
-      <c r="G133" s="8"/>
-      <c r="H133" s="8"/>
-      <c r="I133" s="8"/>
-      <c r="J133" s="8"/>
-      <c r="K133" s="8"/>
-      <c r="L133" s="8"/>
+    <row r="133" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M133" s="3" t="s">
         <v>282</v>
       </c>
@@ -9186,19 +8351,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="134" spans="1:31" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="8"/>
-      <c r="B134" s="8"/>
-      <c r="C134" s="8"/>
-      <c r="D134" s="8"/>
-      <c r="E134" s="8"/>
-      <c r="F134" s="8"/>
-      <c r="G134" s="8"/>
-      <c r="H134" s="8"/>
-      <c r="I134" s="8"/>
-      <c r="J134" s="8"/>
-      <c r="K134" s="8"/>
-      <c r="L134" s="8"/>
+    <row r="134" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:30">
       <c r="M134" s="3" t="s">
         <v>285</v>
       </c>
@@ -9248,7 +8401,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="135" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="135" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A135" s="2" t="s">
         <v>288</v>
       </c>
@@ -9283,19 +8436,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="7"/>
-      <c r="B136" s="8"/>
-      <c r="C136" s="8"/>
-      <c r="D136" s="8"/>
-      <c r="E136" s="8"/>
-      <c r="F136" s="8"/>
-      <c r="G136" s="8"/>
-      <c r="H136" s="8"/>
-      <c r="I136" s="8"/>
-      <c r="J136" s="8"/>
-      <c r="K136" s="8"/>
-      <c r="L136" s="8"/>
+    <row r="136" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A136" s="2"/>
       <c r="M136" s="3" t="s">
         <v>288</v>
       </c>
@@ -9327,7 +8469,7 @@
         <v>0</v>
       </c>
       <c r="X136" s="3">
-        <v>1.8446744073709601E+19</v>
+        <v>1.84467440737096e+19</v>
       </c>
       <c r="Y136" s="3" t="s">
         <v>49</v>
@@ -9339,7 +8481,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="137" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A137" s="2" t="s">
         <v>290</v>
       </c>
@@ -9374,19 +8516,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="7"/>
-      <c r="B138" s="8"/>
-      <c r="C138" s="8"/>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8"/>
-      <c r="F138" s="8"/>
-      <c r="G138" s="8"/>
-      <c r="H138" s="8"/>
-      <c r="I138" s="8"/>
-      <c r="J138" s="8"/>
-      <c r="K138" s="8"/>
-      <c r="L138" s="8"/>
+    <row r="138" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A138" s="2"/>
       <c r="M138" s="3" t="s">
         <v>290</v>
       </c>
@@ -9418,7 +8549,7 @@
         <v>0</v>
       </c>
       <c r="X138" s="3">
-        <v>1.8446744073709601E+19</v>
+        <v>1.84467440737096e+19</v>
       </c>
       <c r="Y138" s="3" t="s">
         <v>49</v>
@@ -9430,7 +8561,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="139" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="139" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A139" s="2" t="s">
         <v>292</v>
       </c>
@@ -9465,19 +8596,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:31" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="7"/>
-      <c r="B140" s="8"/>
-      <c r="C140" s="8"/>
-      <c r="D140" s="8"/>
-      <c r="E140" s="8"/>
-      <c r="F140" s="8"/>
-      <c r="G140" s="8"/>
-      <c r="H140" s="8"/>
-      <c r="I140" s="8"/>
-      <c r="J140" s="8"/>
-      <c r="K140" s="8"/>
-      <c r="L140" s="8"/>
+    <row r="140" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A140" s="2"/>
       <c r="M140" s="3" t="s">
         <v>294</v>
       </c>
@@ -9527,19 +8647,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="141" spans="1:31" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A141" s="8"/>
-      <c r="B141" s="8"/>
-      <c r="C141" s="8"/>
-      <c r="D141" s="8"/>
-      <c r="E141" s="8"/>
-      <c r="F141" s="8"/>
-      <c r="G141" s="8"/>
-      <c r="H141" s="8"/>
-      <c r="I141" s="8"/>
-      <c r="J141" s="8"/>
-      <c r="K141" s="8"/>
-      <c r="L141" s="8"/>
+    <row r="141" s="3" customFormat="1" ht="60" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M141" s="3" t="s">
         <v>297</v>
       </c>
@@ -9589,19 +8697,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="142" spans="1:31" s="3" customFormat="1" ht="240" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="8"/>
-      <c r="B142" s="8"/>
-      <c r="C142" s="8"/>
-      <c r="D142" s="8"/>
-      <c r="E142" s="8"/>
-      <c r="F142" s="8"/>
-      <c r="G142" s="8"/>
-      <c r="H142" s="8"/>
-      <c r="I142" s="8"/>
-      <c r="J142" s="8"/>
-      <c r="K142" s="8"/>
-      <c r="L142" s="8"/>
+    <row r="142" s="3" customFormat="1" ht="240" hidden="1" outlineLevel="1" spans="13:31">
       <c r="M142" s="3" t="s">
         <v>300</v>
       </c>
@@ -9651,7 +8747,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="143" spans="1:31" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="143" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A143" s="2" t="s">
         <v>303</v>
       </c>
@@ -9686,19 +8782,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:31" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="7"/>
-      <c r="B144" s="8"/>
-      <c r="C144" s="8"/>
-      <c r="D144" s="8"/>
-      <c r="E144" s="8"/>
-      <c r="F144" s="8"/>
-      <c r="G144" s="8"/>
-      <c r="H144" s="8"/>
-      <c r="I144" s="8"/>
-      <c r="J144" s="8"/>
-      <c r="K144" s="8"/>
-      <c r="L144" s="8"/>
+    <row r="144" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="1:31">
+      <c r="A144" s="2"/>
       <c r="M144" s="3" t="s">
         <v>305</v>
       </c>
@@ -9748,7 +8833,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="145" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="145" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A145" s="2" t="s">
         <v>308</v>
       </c>
@@ -9783,19 +8868,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A146" s="7"/>
-      <c r="B146" s="8"/>
-      <c r="C146" s="8"/>
-      <c r="D146" s="8"/>
-      <c r="E146" s="8"/>
-      <c r="F146" s="8"/>
-      <c r="G146" s="8"/>
-      <c r="H146" s="8"/>
-      <c r="I146" s="8"/>
-      <c r="J146" s="8"/>
-      <c r="K146" s="8"/>
-      <c r="L146" s="8"/>
+    <row r="146" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A146" s="2"/>
       <c r="M146" s="3" t="s">
         <v>311</v>
       </c>
@@ -9842,19 +8916,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:27" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="8"/>
-      <c r="B147" s="8"/>
-      <c r="C147" s="8"/>
-      <c r="D147" s="8"/>
-      <c r="E147" s="8"/>
-      <c r="F147" s="8"/>
-      <c r="G147" s="8"/>
-      <c r="H147" s="8"/>
-      <c r="I147" s="8"/>
-      <c r="J147" s="8"/>
-      <c r="K147" s="8"/>
-      <c r="L147" s="8"/>
+    <row r="147" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M147" s="3" t="s">
         <v>312</v>
       </c>
@@ -9901,19 +8963,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="148" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="8"/>
-      <c r="B148" s="8"/>
-      <c r="C148" s="8"/>
-      <c r="D148" s="8"/>
-      <c r="E148" s="8"/>
-      <c r="F148" s="8"/>
-      <c r="G148" s="8"/>
-      <c r="H148" s="8"/>
-      <c r="I148" s="8"/>
-      <c r="J148" s="8"/>
-      <c r="K148" s="8"/>
-      <c r="L148" s="8"/>
+    <row r="148" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M148" s="3" t="s">
         <v>313</v>
       </c>
@@ -9960,19 +9010,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="8"/>
-      <c r="B149" s="8"/>
-      <c r="C149" s="8"/>
-      <c r="D149" s="8"/>
-      <c r="E149" s="8"/>
-      <c r="F149" s="8"/>
-      <c r="G149" s="8"/>
-      <c r="H149" s="8"/>
-      <c r="I149" s="8"/>
-      <c r="J149" s="8"/>
-      <c r="K149" s="8"/>
-      <c r="L149" s="8"/>
+    <row r="149" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M149" s="3" t="s">
         <v>314</v>
       </c>
@@ -10019,19 +9057,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="150" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="8"/>
-      <c r="B150" s="8"/>
-      <c r="C150" s="8"/>
-      <c r="D150" s="8"/>
-      <c r="E150" s="8"/>
-      <c r="F150" s="8"/>
-      <c r="G150" s="8"/>
-      <c r="H150" s="8"/>
-      <c r="I150" s="8"/>
-      <c r="J150" s="8"/>
-      <c r="K150" s="8"/>
-      <c r="L150" s="8"/>
+    <row r="150" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M150" s="3" t="s">
         <v>315</v>
       </c>
@@ -10078,7 +9104,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="151" spans="1:27" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" x14ac:dyDescent="0.25">
+    <row r="151" s="2" customFormat="1" ht="24" customHeight="1" collapsed="1" spans="1:11">
       <c r="A151" s="2" t="s">
         <v>316</v>
       </c>
@@ -10113,19 +9139,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A152" s="7"/>
-      <c r="B152" s="8"/>
-      <c r="C152" s="8"/>
-      <c r="D152" s="8"/>
-      <c r="E152" s="8"/>
-      <c r="F152" s="8"/>
-      <c r="G152" s="8"/>
-      <c r="H152" s="8"/>
-      <c r="I152" s="8"/>
-      <c r="J152" s="8"/>
-      <c r="K152" s="8"/>
-      <c r="L152" s="8"/>
+    <row r="152" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="1:27">
+      <c r="A152" s="2"/>
       <c r="M152" s="3" t="s">
         <v>319</v>
       </c>
@@ -10172,19 +9187,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="153" spans="1:27" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A153" s="8"/>
-      <c r="B153" s="8"/>
-      <c r="C153" s="8"/>
-      <c r="D153" s="8"/>
-      <c r="E153" s="8"/>
-      <c r="F153" s="8"/>
-      <c r="G153" s="8"/>
-      <c r="H153" s="8"/>
-      <c r="I153" s="8"/>
-      <c r="J153" s="8"/>
-      <c r="K153" s="8"/>
-      <c r="L153" s="8"/>
+    <row r="153" s="3" customFormat="1" ht="30" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M153" s="3" t="s">
         <v>320</v>
       </c>
@@ -10231,19 +9234,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="154" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A154" s="8"/>
-      <c r="B154" s="8"/>
-      <c r="C154" s="8"/>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8"/>
-      <c r="F154" s="8"/>
-      <c r="G154" s="8"/>
-      <c r="H154" s="8"/>
-      <c r="I154" s="8"/>
-      <c r="J154" s="8"/>
-      <c r="K154" s="8"/>
-      <c r="L154" s="8"/>
+    <row r="154" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M154" s="3" t="s">
         <v>321</v>
       </c>
@@ -10290,19 +9281,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="8"/>
-      <c r="B155" s="8"/>
-      <c r="C155" s="8"/>
-      <c r="D155" s="8"/>
-      <c r="E155" s="8"/>
-      <c r="F155" s="8"/>
-      <c r="G155" s="8"/>
-      <c r="H155" s="8"/>
-      <c r="I155" s="8"/>
-      <c r="J155" s="8"/>
-      <c r="K155" s="8"/>
-      <c r="L155" s="8"/>
+    <row r="155" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M155" s="3" t="s">
         <v>322</v>
       </c>
@@ -10349,19 +9328,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="156" spans="1:27" s="3" customFormat="1" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A156" s="8"/>
-      <c r="B156" s="8"/>
-      <c r="C156" s="8"/>
-      <c r="D156" s="8"/>
-      <c r="E156" s="8"/>
-      <c r="F156" s="8"/>
-      <c r="G156" s="8"/>
-      <c r="H156" s="8"/>
-      <c r="I156" s="8"/>
-      <c r="J156" s="8"/>
-      <c r="K156" s="8"/>
-      <c r="L156" s="8"/>
+    <row r="156" s="3" customFormat="1" hidden="1" outlineLevel="1" spans="13:27">
       <c r="M156" s="3" t="s">
         <v>323</v>
       </c>
@@ -10410,15 +9377,20 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="A136:L136"/>
+    <mergeCell ref="A138:L138"/>
+    <mergeCell ref="A144:L144"/>
     <mergeCell ref="A152:L156"/>
     <mergeCell ref="A109:L116"/>
     <mergeCell ref="A118:L125"/>
     <mergeCell ref="A127:L134"/>
     <mergeCell ref="A140:L142"/>
     <mergeCell ref="A146:L150"/>
-    <mergeCell ref="A136:L136"/>
-    <mergeCell ref="A138:L138"/>
-    <mergeCell ref="A144:L144"/>
     <mergeCell ref="A7:L11"/>
     <mergeCell ref="A13:L23"/>
     <mergeCell ref="A31:L35"/>
@@ -10432,13 +9404,8 @@
     <mergeCell ref="A82:L89"/>
     <mergeCell ref="A91:L98"/>
     <mergeCell ref="A100:L107"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="A29:L29"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>